<commit_message>
1.  完善 LevelChoicePanel 2. 增加 ObjectPool 模块
</commit_message>
<xml_diff>
--- a/Egg/Luban/Configs/Datas/#LevelData.xlsx
+++ b/Egg/Luban/Configs/Datas/#LevelData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20670" windowHeight="13815"/>
+    <workbookView windowHeight="17775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>##var</t>
   </si>
@@ -118,7 +118,7 @@
     </r>
   </si>
   <si>
-    <t>level</t>
+    <t>path</t>
   </si>
   <si>
     <t>levelType</t>
@@ -133,6 +133,9 @@
     <t>int</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>Level.GameType</t>
   </si>
   <si>
@@ -155,6 +158,96 @@
   </si>
   <si>
     <t>锁定方式</t>
+  </si>
+  <si>
+    <t>Level_001</t>
+  </si>
+  <si>
+    <t>Level_002</t>
+  </si>
+  <si>
+    <t>Level_003</t>
+  </si>
+  <si>
+    <t>Level_004</t>
+  </si>
+  <si>
+    <t>Level_005</t>
+  </si>
+  <si>
+    <t>Level_006</t>
+  </si>
+  <si>
+    <t>Level_007</t>
+  </si>
+  <si>
+    <t>Level_008</t>
+  </si>
+  <si>
+    <t>Level_009</t>
+  </si>
+  <si>
+    <t>Level_010</t>
+  </si>
+  <si>
+    <t>Level_011</t>
+  </si>
+  <si>
+    <t>Level_012</t>
+  </si>
+  <si>
+    <t>Level_013</t>
+  </si>
+  <si>
+    <t>Level_014</t>
+  </si>
+  <si>
+    <t>Level_015</t>
+  </si>
+  <si>
+    <t>Level_016</t>
+  </si>
+  <si>
+    <t>Level_017</t>
+  </si>
+  <si>
+    <t>Level_018</t>
+  </si>
+  <si>
+    <t>Level_019</t>
+  </si>
+  <si>
+    <t>Level_020</t>
+  </si>
+  <si>
+    <t>Level_021</t>
+  </si>
+  <si>
+    <t>Level_022</t>
+  </si>
+  <si>
+    <t>Level_023</t>
+  </si>
+  <si>
+    <t>Level_024</t>
+  </si>
+  <si>
+    <t>Level_025</t>
+  </si>
+  <si>
+    <t>Level_026</t>
+  </si>
+  <si>
+    <t>Level_027</t>
+  </si>
+  <si>
+    <t>Level_028</t>
+  </si>
+  <si>
+    <t>Level_029</t>
+  </si>
+  <si>
+    <t>Level_030</t>
   </si>
 </sst>
 </file>
@@ -816,7 +909,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -828,11 +921,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
@@ -1151,276 +1262,276 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="24.6583333333333" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.6583333333333" style="5" customWidth="1"/>
     <col min="5" max="5" width="17.45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="14">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="14">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="14">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="14">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="14">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="14">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="14">
         <v>9</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:5">
+      <c r="B15" s="15">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="14">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="14">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="14">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="14">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="8">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="8">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10" s="8">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" s="8">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" s="8">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="8">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" s="8">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>9</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:5">
-      <c r="B15" s="9">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="8">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>11</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="8">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="8">
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="8">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5">
         <v>0</v>
       </c>
       <c r="E19">
@@ -1428,13 +1539,13 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="8">
+      <c r="B20" s="14">
         <v>15</v>
       </c>
-      <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="5">
         <v>0</v>
       </c>
       <c r="E20">
@@ -1442,13 +1553,13 @@
       </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="2:5">
-      <c r="B21" s="9">
+      <c r="B21" s="15">
         <v>16</v>
       </c>
-      <c r="C21" s="1">
-        <v>16</v>
-      </c>
-      <c r="D21">
+      <c r="C21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="5">
         <v>0</v>
       </c>
       <c r="E21">
@@ -1456,13 +1567,13 @@
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="8">
+      <c r="B22" s="14">
         <v>17</v>
       </c>
-      <c r="C22">
-        <v>17</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="5">
         <v>0</v>
       </c>
       <c r="E22">
@@ -1470,13 +1581,13 @@
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="8">
+      <c r="B23" s="14">
         <v>18</v>
       </c>
-      <c r="C23">
-        <v>18</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5">
         <v>0</v>
       </c>
       <c r="E23">
@@ -1484,13 +1595,13 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="8">
+      <c r="B24" s="14">
         <v>19</v>
       </c>
-      <c r="C24">
-        <v>19</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="5">
         <v>0</v>
       </c>
       <c r="E24">
@@ -1498,13 +1609,13 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="8">
+      <c r="B25" s="14">
         <v>20</v>
       </c>
-      <c r="C25">
-        <v>20</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="5">
         <v>0</v>
       </c>
       <c r="E25">
@@ -1512,13 +1623,13 @@
       </c>
     </row>
     <row r="26" s="1" customFormat="1" spans="2:5">
-      <c r="B26" s="9">
+      <c r="B26" s="15">
         <v>21</v>
       </c>
-      <c r="C26" s="1">
-        <v>21</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="5">
         <v>0</v>
       </c>
       <c r="E26">
@@ -1526,13 +1637,13 @@
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="8">
+      <c r="B27" s="14">
         <v>22</v>
       </c>
-      <c r="C27">
-        <v>22</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="5">
         <v>0</v>
       </c>
       <c r="E27">
@@ -1540,13 +1651,13 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="8">
+      <c r="B28" s="14">
         <v>23</v>
       </c>
-      <c r="C28">
-        <v>23</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="5">
         <v>0</v>
       </c>
       <c r="E28">
@@ -1554,13 +1665,13 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="8">
+      <c r="B29" s="14">
         <v>24</v>
       </c>
-      <c r="C29">
-        <v>24</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="5">
         <v>0</v>
       </c>
       <c r="E29">
@@ -1568,13 +1679,13 @@
       </c>
     </row>
     <row r="30" s="2" customFormat="1" spans="2:5">
-      <c r="B30" s="8">
+      <c r="B30" s="14">
         <v>25</v>
       </c>
-      <c r="C30" s="2">
-        <v>25</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="5">
         <v>0</v>
       </c>
       <c r="E30">
@@ -1582,13 +1693,13 @@
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="13" customHeight="1" spans="2:5">
-      <c r="B31" s="9">
+      <c r="B31" s="15">
         <v>26</v>
       </c>
-      <c r="C31" s="1">
-        <v>26</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="5">
         <v>0</v>
       </c>
       <c r="E31">
@@ -1596,13 +1707,13 @@
       </c>
     </row>
     <row r="32" s="2" customFormat="1" spans="2:5">
-      <c r="B32" s="8">
+      <c r="B32" s="14">
         <v>27</v>
       </c>
-      <c r="C32" s="2">
-        <v>27</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="5">
         <v>0</v>
       </c>
       <c r="E32">
@@ -1610,13 +1721,13 @@
       </c>
     </row>
     <row r="33" s="2" customFormat="1" spans="2:5">
-      <c r="B33" s="8">
+      <c r="B33" s="14">
         <v>28</v>
       </c>
-      <c r="C33" s="2">
-        <v>28</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="5">
         <v>0</v>
       </c>
       <c r="E33">
@@ -1624,13 +1735,13 @@
       </c>
     </row>
     <row r="34" s="2" customFormat="1" spans="2:5">
-      <c r="B34" s="8">
+      <c r="B34" s="14">
         <v>29</v>
       </c>
-      <c r="C34" s="2">
-        <v>29</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="5">
         <v>0</v>
       </c>
       <c r="E34">
@@ -1638,39 +1749,99 @@
       </c>
     </row>
     <row r="35" s="2" customFormat="1" spans="2:5">
-      <c r="B35" s="8">
+      <c r="B35" s="14">
         <v>30</v>
       </c>
-      <c r="C35" s="2">
-        <v>30</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="5">
         <v>0</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="1"/>
-    <row r="37" customFormat="1"/>
-    <row r="38" customFormat="1"/>
-    <row r="39" customFormat="1"/>
-    <row r="40" customFormat="1"/>
-    <row r="41" customFormat="1"/>
-    <row r="42" customFormat="1"/>
-    <row r="43" customFormat="1"/>
-    <row r="44" customFormat="1"/>
-    <row r="45" customFormat="1"/>
-    <row r="46" customFormat="1"/>
-    <row r="47" customFormat="1"/>
-    <row r="48" customFormat="1"/>
-    <row r="49" customFormat="1"/>
-    <row r="50" customFormat="1"/>
-    <row r="51" customFormat="1"/>
-    <row r="52" customFormat="1"/>
-    <row r="53" customFormat="1"/>
-    <row r="54" customFormat="1"/>
-    <row r="55" customFormat="1"/>
+    <row r="36" customFormat="1" spans="2:5">
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" customFormat="1" spans="2:5">
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" customFormat="1" spans="2:5">
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" customFormat="1" spans="2:5">
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" customFormat="1" spans="2:5">
+      <c r="C40" s="4"/>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" customFormat="1" spans="2:5">
+      <c r="C41" s="4"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" customFormat="1" spans="2:5">
+      <c r="C42" s="4"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" customFormat="1" spans="2:5">
+      <c r="C43" s="4"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" customFormat="1" spans="2:5">
+      <c r="C44" s="4"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" customFormat="1" spans="2:5">
+      <c r="C45" s="4"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" customFormat="1" spans="2:5">
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" customFormat="1" spans="2:5">
+      <c r="C47" s="4"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" customFormat="1" spans="2:5">
+      <c r="C48" s="4"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49" customFormat="1" spans="3:4">
+      <c r="C49" s="4"/>
+      <c r="D49" s="5"/>
+    </row>
+    <row r="50" customFormat="1" spans="3:4">
+      <c r="C50" s="4"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" customFormat="1" spans="3:4">
+      <c r="C51" s="4"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" customFormat="1" spans="3:4">
+      <c r="C52" s="4"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" customFormat="1" spans="3:4">
+      <c r="C53" s="4"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" customFormat="1" spans="3:4">
+      <c r="C54" s="4"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" customFormat="1" spans="3:4">
+      <c r="C55" s="4"/>
+      <c r="D55" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>